<commit_message>
Add thêm file reference về report và software requirement của nhóm khác
</commit_message>
<xml_diff>
--- a/Teamwork/Project member.xlsx
+++ b/Teamwork/Project member.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\VPS-Monitor\Teamwork\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="60" windowWidth="20340" windowHeight="7875"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
   <si>
     <t>Lê Thị Thu Hà</t>
     <phoneticPr fontId="1"/>
@@ -159,23 +164,50 @@
     <t>Role and Responsibility</t>
     <phoneticPr fontId="1"/>
   </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Ngày</t>
+  </si>
+  <si>
+    <t>Thành viên</t>
+  </si>
+  <si>
+    <t>Miss</t>
+  </si>
+  <si>
+    <t>Huỳnh Hiếu Bảo</t>
+  </si>
+  <si>
+    <t>Yêu cầu tạo tài khoản FB và gửi cho Hà cũng chưa gửi, Nhắn các bạn set up môi trường, cài Slack mà vẫn chưa thấy tài khoản của Bảo join vào group. Ngày đầu tiên vì bận mà ko đến được cũng không gọi điện chủ động nói, mà đợi Hà gọi mới biết là Bảo ko đến được</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Sáng hoặc chiều</t>
+  </si>
+  <si>
+    <t>Từ 10h30 trở đi</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="6"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -184,7 +216,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -232,7 +264,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -255,6 +287,102 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -264,7 +392,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -283,26 +411,244 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="ハイパーリンク" xfId="1" builtinId="8"/>
-    <cellStyle name="標準" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="8">
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Cambria"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Cambria"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A4:D8" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
+  <autoFilter ref="A4:D8"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="No" dataDxfId="3"/>
+    <tableColumn id="2" name="Ngày" dataDxfId="2"/>
+    <tableColumn id="3" name="Thành viên" dataDxfId="1"/>
+    <tableColumn id="4" name="Miss" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office ​​テーマ">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -344,7 +690,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -379,7 +725,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -588,40 +934,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection sqref="A1:F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="9" style="2"/>
     <col min="2" max="3" width="19.75" style="2" customWidth="1"/>
     <col min="4" max="5" width="13.75" style="2" customWidth="1"/>
     <col min="6" max="6" width="32.5" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="9" style="2"/>
+    <col min="7" max="7" width="16.75" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:7">
+      <c r="A1" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-    </row>
-    <row r="4" spans="1:6" ht="18" x14ac:dyDescent="0.15">
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="20"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+    </row>
+    <row r="4" spans="1:7" ht="18">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -640,8 +987,11 @@
       <c r="F4" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G4" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" s="3">
         <v>1</v>
       </c>
@@ -657,7 +1007,7 @@
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7">
       <c r="A6" s="3">
         <v>2</v>
       </c>
@@ -676,8 +1026,11 @@
       <c r="F6" s="5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G6" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" s="3">
         <v>3</v>
       </c>
@@ -696,8 +1049,11 @@
       <c r="F7" s="5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G7" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" s="3">
         <v>4</v>
       </c>
@@ -717,7 +1073,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7">
       <c r="A9" s="3">
         <v>5</v>
       </c>
@@ -735,6 +1091,9 @@
       </c>
       <c r="F9" s="5" t="s">
         <v>7</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -755,14 +1114,80 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A4:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="2" max="2" width="14.125" customWidth="1"/>
+    <col min="3" max="3" width="20.75" customWidth="1"/>
+    <col min="4" max="4" width="62.25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="1:4" s="18" customFormat="1">
+      <c r="A4" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="68.25" customHeight="1">
+      <c r="A5" s="7">
+        <v>1</v>
+      </c>
+      <c r="B5" s="14">
+        <v>42373</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="7">
+        <v>2</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="9"/>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="7">
+        <v>3</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="9"/>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="10">
+        <v>4</v>
+      </c>
+      <c r="B8" s="11"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="13"/>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="6"/>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -772,7 +1197,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData/>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>